<commit_message>
hours update and TAR update
</commit_message>
<xml_diff>
--- a/status reports/david.xlsx
+++ b/status reports/david.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -108,6 +108,10 @@
   </si>
   <si>
     <t>1/21/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/26/2010</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -467,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -665,6 +669,28 @@
       </c>
       <c r="C17" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update source add
</commit_message>
<xml_diff>
--- a/status reports/david.xlsx
+++ b/status reports/david.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -123,6 +123,10 @@
   </si>
   <si>
     <t>Solid Modeling of design (span of reading break)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Group Meeting</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -493,7 +497,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -988,10 +992,26 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2">
+        <v>40260</v>
+      </c>
+      <c r="B45">
+        <v>2.5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2">
+        <v>40260</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2"/>

</xml_diff>